<commit_message>
sync (this will not be permenant)
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -651,12 +651,13 @@
 Merged: Feat: FF to control late subscription alert</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" xml:space="preserve">
       <c r="A23" t="str">
-        <v>2024-02-06</v>
-      </c>
-      <c r="B23" t="str">
-        <v>Created: Feat: Test PR</v>
+        <v>2024-02-07</v>
+      </c>
+      <c r="B23" t="str" xml:space="preserve">
+        <v xml:space="preserve">Created: Fix: Action filters default enabled, Fix: All actions ticked by default
+Closed: Fix: All actions ticked by default</v>
       </c>
       <c r="C23" t="str">
         <v/>

</xml_diff>

<commit_message>
Created function to derive skills from the pr
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -659,14 +659,57 @@
         <v xml:space="preserve">Created: Fix: Action filters default enabled, Fix: All actions ticked by default
 Closed: Fix: All actions ticked by default</v>
       </c>
-      <c r="C23" t="str">
-        <v/>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>2024-02-12</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Created: Fix: Spacing discrepancy on share report modal</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>2024-02-16</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Worked on: Feat: Open Weather Integration</v>
+      </c>
+    </row>
+    <row r="26" xml:space="preserve">
+      <c r="A26" t="str">
+        <v>2024-02-19</v>
+      </c>
+      <c r="B26" t="str" xml:space="preserve">
+        <v xml:space="preserve">Worked on: Fix: Action filters default enabled
+Merged: Fix: Action filters default enabled</v>
+      </c>
+    </row>
+    <row r="27" xml:space="preserve">
+      <c r="A27" t="str">
+        <v>2024-02-20</v>
+      </c>
+      <c r="B27" t="str" xml:space="preserve">
+        <v xml:space="preserve">Worked on: Feat: Visual password feedback on password forget screen, Feat: Custom field activities and create activites on update/create
+Merged: Feat: Visual password feedback on password forget screen</v>
+      </c>
+    </row>
+    <row r="28" xml:space="preserve">
+      <c r="A28" t="str">
+        <v>2024-02-21</v>
+      </c>
+      <c r="B28" t="str" xml:space="preserve">
+        <v xml:space="preserve">Worked on: Feat: Custom field activities and create activites on update/create
+Created: Fix: Additional email sending on inspection close</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Improved my PHP, PHPUnit, Typescript, PHPSpec, and Laravel skills</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D28"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>